<commit_message>
ajout outils et autres petites modifications
</commit_message>
<xml_diff>
--- a/cours.xlsx
+++ b/cours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/projets/techinfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13375412-202A-034A-A09D-FECD1F155DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12932275-0A16-B64D-AA06-A2664DE0EEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{643C1454-08AC-524D-90A3-F7CC1ACD2A43}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Cours</t>
   </si>
@@ -235,12 +235,40 @@
   <si>
     <t>Titre</t>
   </si>
+  <si>
+    <t>Cible de formation</t>
+  </si>
+  <si>
+    <t>À la fin du cours, l’élève sera capable d’analyser des problèmes contextuels d’informatique à partir de situations problèmes et de données quantitatives ainsi que de les résoudre en traitant les nombres à représenter dans la mémoire d’un ordinateur et en modélisant les raisonnements logiques à plusieurs variables.</t>
+  </si>
+  <si>
+    <t>À la fin du cours l'élève sera capable, dans un environnement ergonomique, de préparer un ordinateur et d'en faire l'installation. Il sera aussi en mesure d’installer le système d'exploitation ainsi que les logiciels requis.</t>
+  </si>
+  <si>
+    <t>À la fin du cours, l'élève sera capable de traiter l’information relative aux réalités du milieu du travail en informatique en utilisant le système d’exploitation macOS et les logiciels de bureautique infonuagiques</t>
+  </si>
+  <si>
+    <t>À la fin du cours, l'élève sera capable de résoudre des problèmes simples en traduisant des algorithmes dans un langage de programmation.</t>
+  </si>
+  <si>
+    <t>À la fin du cours, l'élève sera capable d'effectuer le développement côté client pour des applications Web.</t>
+  </si>
+  <si>
+    <t>À la fin de ce cours, l'élève sera capable d'effectuer le développement d’applications Web transactionnelles.</t>
+  </si>
+  <si>
+    <t>Cours préalables</t>
+  </si>
+  <si>
+    <t>420-1D6-VI : Programmation 1 
+420-1E6-VI : Design Web</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -273,6 +301,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
+      <name val="PT Sans"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -294,12 +329,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,8 +515,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -523,8 +564,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -571,8 +612,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -764,8 +805,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -813,8 +854,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -861,8 +902,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1199,8 +1240,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1248,8 +1289,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1296,8 +1337,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1489,8 +1530,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1538,8 +1579,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1586,8 +1627,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1779,8 +1820,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1828,8 +1869,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1876,8 +1917,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2069,8 +2110,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2118,8 +2159,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2166,8 +2207,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2359,8 +2400,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2408,8 +2449,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2456,8 +2497,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -24979,75 +25020,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A91030F-DD86-2042-B290-CE7625F78EDF}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.33203125" customWidth="1"/>
+    <col min="3" max="3" width="78.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -25055,7 +25125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -25063,7 +25133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -25071,7 +25141,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -25079,7 +25149,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -25087,7 +25157,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -25095,7 +25165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -25103,7 +25173,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -25111,7 +25181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -25529,6 +25599,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>